<commit_message>
Fixed the missing DOI issue of USENIX papers
</commit_message>
<xml_diff>
--- a/examples/tee/papers_results.xlsx
+++ b/examples/tee/papers_results.xlsx
@@ -1727,6 +1727,11 @@
           <t>mmWall: A Steerable, Transflective Metamaterial Surface for NextG mmWave Networks.</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/nsdi23/presentation/cho-kun-woo</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4655,6 +4660,11 @@
           <t>Trust Dies in Darkness: Shedding Light on Samsung's TrustZone Keymaster Design.</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity22/presentation/shakevsky</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -4685,6 +4695,11 @@
           <t>Pool Inference Attacks on Local Differential Privacy: Quantifying the Privacy Guarantees of Apple's Count Mean Sketch in Practice.</t>
         </is>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity22/presentation/gadotti</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -4715,6 +4730,11 @@
           <t>ReZone: Disarming TrustZone with TEE Privilege Reduction.</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity22/presentation/cerdeira</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -4745,6 +4765,11 @@
           <t>Repurposing Segmentation as a Practical LVI-NULL Mitigation in SGX.</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity22/presentation/giner</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -4775,6 +4800,11 @@
           <t>SGXFuzz: Efficiently Synthesizing Nested Structures for SGX Enclave Fuzzing.</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity22/presentation/cloosters</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -4805,6 +4835,11 @@
           <t>SGXLock: Towards Efficiently Establishing Mutual Distrust Between Host Application and Enclave for SGX.</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity22/presentation/chen-yuan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -4835,6 +4870,11 @@
           <t>Minefield: A Software-only Protection for SGX Enclaves against DVFS Attacks.</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity22/presentation/kogler-minefield</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -4865,6 +4905,11 @@
           <t>Design of Access Control Mechanisms in Systems-on-Chip with Formal Integrity Guarantees.</t>
         </is>
       </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity23/presentation/mehmedagic</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -4895,6 +4940,11 @@
           <t>Fourteen Years in the Life: A Root Server's Perspective on DNS Resolver Security.</t>
         </is>
       </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity23/presentation/hilton</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -4925,6 +4975,11 @@
           <t>Reusable Enclaves for Confidential Serverless Computing.</t>
         </is>
       </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity23/presentation/zhao-shixuan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -4955,6 +5010,11 @@
           <t>AEX-Notify: Thwarting Precise Single-Stepping Attacks through Interrupt Awareness for Intel SGX Enclaves.</t>
         </is>
       </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity23/presentation/constable</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -4985,6 +5045,11 @@
           <t>A Verified Confidential Computing as a Service Framework for Privacy Preservation.</t>
         </is>
       </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity23/presentation/chen-hongbo</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -5015,6 +5080,11 @@
           <t>Extended Hell(o): A Comprehensive Large-Scale Study on Email Confidentiality and Integrity Mechanisms in the Wild.</t>
         </is>
       </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity23/presentation/blechschmidt</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -5045,6 +5115,11 @@
           <t>WaterBear: Practical Asynchronous BFT Matching Security Guarantees of Partially Synchronous BFT.</t>
         </is>
       </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity23/presentation/zhang-haibin</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -5075,6 +5150,11 @@
           <t>ACFA: Secure Runtime Auditing &amp; Guaranteed Device Healing via Active Control Flow Attestation.</t>
         </is>
       </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity23/presentation/caulfield</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -5105,6 +5185,11 @@
           <t>Oops..! I Glitched It Again! How to Multi-Glitch the Glitching-Protections on ARM TrustZone-M.</t>
         </is>
       </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity23/presentation/sass</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -5135,6 +5220,11 @@
           <t>Zero-setup Intermediate-rate Communication Guarantees in a Global Internet.</t>
         </is>
       </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity24/presentation/wyss</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -5165,6 +5255,11 @@
           <t>00SEVen - Re-enabling Virtual Machine Forensics: Introspecting Confidential VMs Using Privileged in-VM Agents.</t>
         </is>
       </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity24/presentation/schwarz</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -5195,6 +5290,11 @@
           <t>ACAI: Protecting Accelerator Execution with Arm Confidential Computing Architecture.</t>
         </is>
       </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity24/presentation/sridhara</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -5225,6 +5325,11 @@
           <t>HECKLER: Breaking Confidential VMs with Malicious Interrupts.</t>
         </is>
       </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity24/presentation/schl%C3%BCter</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -5253,6 +5358,11 @@
       <c r="F22" t="inlineStr">
         <is>
           <t>GlobalConfusion: TrustZone Trusted Application 0-Days by Design.</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/usenixsecurity24/presentation/busch-globalconfusion</t>
         </is>
       </c>
     </row>
@@ -5341,6 +5451,11 @@
           <t>MyTEE: Own the Trusted Execution Environment on Embedded Devices.</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://www.ndss-symposium.org/ndss-paper/mytee-own-the-trusted-execution-environment-on-embedded-devices/</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -5371,6 +5486,11 @@
           <t>RR: A Fault Model for Efficient TEE Replication.</t>
         </is>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>https://www.ndss-symposium.org/ndss-paper/rr-a-fault-model-for-efficient-tee-replication/</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -5401,6 +5521,11 @@
           <t>LDR: Secure and Efficient Linux Driver Runtime for Embedded TEE Systems.</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>https://www.ndss-symposium.org/ndss-paper/ldr-secure-and-efficient-linux-driver-runtime-for-embedded-tee-systems/</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -5431,6 +5556,11 @@
           <t>Overconfidence is a Dangerous Thing: Mitigating Membership Inference Attacks by Enforcing Less Confident Prediction.</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>https://www.ndss-symposium.org/ndss-paper/overconfidence-is-a-dangerous-thing-mitigating-membership-inference-attacks-by-enforcing-less-confident-prediction/</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -5461,6 +5591,11 @@
           <t>EnclaveFuzz: Finding Vulnerabilities in SGX Applications.</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>https://www.ndss-symposium.org/ndss-paper/enclavefuzz-finding-vulnerabilities-in-sgx-applications/</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -5491,6 +5626,11 @@
           <t>Faults in Our Bus: Novel Bus Fault Attack to Break ARM TrustZone.</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>https://www.ndss-symposium.org/ndss-paper/faults-in-our-bus-novel-bus-fault-attack-to-break-arm-trustzone/</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -5521,6 +5661,11 @@
           <t>SENSE: Enhancing Microarchitectural Awareness for TEEs via Subscription-Based Notification.</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>https://www.ndss-symposium.org/ndss-paper/sense-enhancing-microarchitectural-awareness-for-tees-via-subscription-based-notification/</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -5549,6 +5694,11 @@
       <c r="F9" t="inlineStr">
         <is>
           <t>TEE-SHirT: Scalable Leakage-Free Cache Hierarchies for TEEs.</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>https://www.ndss-symposium.org/ndss-paper/tee-shirt-scalable-leakage-free-cache-hierarchies-for-tees/</t>
         </is>
       </c>
     </row>
@@ -7387,6 +7537,11 @@
           <t>Design and Verification of the Arm Confidential Compute Architecture.</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/osdi22/presentation/li</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7417,6 +7572,11 @@
           <t>An Extensible Orchestration and Protection Framework for Confidential Cloud Computing.</t>
         </is>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/osdi23/presentation/ahmad</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7447,6 +7607,11 @@
           <t>Nimble: Rollback Protection for Confidential Cloud Services.</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/osdi23/presentation/angel</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7477,6 +7642,11 @@
           <t>Core slicing: closing the gap between leaky confidential VMs and bare-metal cloud.</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/osdi23/presentation/zhou-ziqiao</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7505,6 +7675,11 @@
       <c r="F6" t="inlineStr">
         <is>
           <t>VeriSMo: A Verified Security Module for Confidential VMs.</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/osdi24/presentation/zhou</t>
         </is>
       </c>
     </row>
@@ -9042,6 +9217,11 @@
           <t>Trustful Data Sharing in the Forest-based Sector - Opportunities and Challenges for a Data Trustee.</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://ceur-ws.org/Vol-3462/DEco1.pdf</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9807,6 +9987,11 @@
           <t>PRIDWEN: Universally Hardening SGX Programs via Load-Time Synthesis.</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/atc22/presentation/sang</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -9837,6 +10022,11 @@
           <t>Bifrost: Analysis and Optimization of Network I/O Tax in Confidential Virtual Machines.</t>
         </is>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/atc23/presentation/li-dingji</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -9867,6 +10057,11 @@
           <t>Confidential Computing within an AI Accelerator.</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/atc23/presentation/vaswani</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -9897,6 +10092,11 @@
           <t>Mangosteen: Fast Transparent Durability for Linearizable Applications using NVM.</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/atc24/presentation/egorov</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -9925,6 +10125,11 @@
       <c r="F6" t="inlineStr">
         <is>
           <t>CPC: Flexible, Secure, and Efficient CVM Maintenance with Confidential Procedure Calls.</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>https://www.usenix.org/conference/atc24/presentation/chen-jiahao</t>
         </is>
       </c>
     </row>

</xml_diff>